<commit_message>
ZSS-576: 1. Range.protectSheet(password, allowXxx, ...), Range.unprotectSheet(), Range.isSheetProtected(), Range.getSheetProtection() 2. Check protection on action 3. Test cases
</commit_message>
<xml_diff>
--- a/zssmodel/src_test/org/zkoss/zss/model/book/import.xlsx
+++ b/zssmodel/src_test/org/zkoss/zss/model/book/import.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-15" yWindow="-15" windowWidth="12720" windowHeight="12975" activeTab="7"/>
+    <workbookView xWindow="-15" yWindow="-15" windowWidth="12720" windowHeight="12975" tabRatio="778" firstSheet="3" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="Value" sheetId="2" r:id="rId1"/>
@@ -15,6 +15,8 @@
     <sheet name="Format" sheetId="6" r:id="rId6"/>
     <sheet name="sheet-protection" sheetId="7" r:id="rId7"/>
     <sheet name="Validation" sheetId="8" r:id="rId8"/>
+    <sheet name="sheet-protection-all" sheetId="11" r:id="rId9"/>
+    <sheet name="sheet-protection-none" sheetId="10" r:id="rId10"/>
   </sheets>
   <definedNames>
     <definedName name="RangeMerged">NamedRange!$F$2</definedName>
@@ -25,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="159">
   <si>
     <t>The first column is freezed.</t>
   </si>
@@ -465,6 +467,57 @@
   </si>
   <si>
     <t>percetage</t>
+  </si>
+  <si>
+    <t>* Select locked cell</t>
+  </si>
+  <si>
+    <t>* Select unlocked cell</t>
+  </si>
+  <si>
+    <t>* Format rows</t>
+  </si>
+  <si>
+    <t>* Format cells</t>
+  </si>
+  <si>
+    <t>* Format columns</t>
+  </si>
+  <si>
+    <t>* Insert columns</t>
+  </si>
+  <si>
+    <t>* Insert rows</t>
+  </si>
+  <si>
+    <t>* Insert hyperlinks</t>
+  </si>
+  <si>
+    <t>* Delete columns</t>
+  </si>
+  <si>
+    <t>* Delete rows</t>
+  </si>
+  <si>
+    <t>* Sort</t>
+  </si>
+  <si>
+    <t>* Use AutoFilter</t>
+  </si>
+  <si>
+    <t>* Use PivotTable reports</t>
+  </si>
+  <si>
+    <t>* Edit objects</t>
+  </si>
+  <si>
+    <t>* Edit scenarios</t>
+  </si>
+  <si>
+    <t>This sheet is protected with none of the following items checked(password: "abc")</t>
+  </si>
+  <si>
+    <t>This sheet is protected with ALL of the following items checked(password: "")</t>
   </si>
 </sst>
 </file>
@@ -1876,6 +1929,102 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:A16"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1">
+      <c r="A3" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1">
+      <c r="A4" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1">
+      <c r="A5" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1">
+      <c r="A6" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1">
+      <c r="A7" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1">
+      <c r="A8" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1">
+      <c r="A9" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1">
+      <c r="A10" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1">
+      <c r="A11" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1">
+      <c r="A12" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1">
+      <c r="A13" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1">
+      <c r="A14" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1">
+      <c r="A15" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1">
+      <c r="A16" t="s">
+        <v>156</v>
+      </c>
+    </row>
+  </sheetData>
+  <sheetProtection password="CC1A" sheet="1" objects="1" scenarios="1" selectLockedCells="1" selectUnlockedCells="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:M38"/>
@@ -3596,7 +3745,7 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection sqref="A1:E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3633,7 +3782,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
@@ -3759,4 +3908,98 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:A16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1">
+      <c r="A3" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1">
+      <c r="A4" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1">
+      <c r="A5" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1">
+      <c r="A6" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1">
+      <c r="A7" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1">
+      <c r="A8" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1">
+      <c r="A9" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1">
+      <c r="A10" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1">
+      <c r="A11" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1">
+      <c r="A12" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1">
+      <c r="A13" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1">
+      <c r="A14" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1">
+      <c r="A15" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1">
+      <c r="A16" t="s">
+        <v>156</v>
+      </c>
+    </row>
+  </sheetData>
+  <sheetProtection sheet="1" formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>